<commit_message>
there are many new graphics here
</commit_message>
<xml_diff>
--- a/chicagoavelsd-4/chicagoavelsd-4.xlsx
+++ b/chicagoavelsd-4/chicagoavelsd-4.xlsx
@@ -38,9 +38,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>subhed</t>
-  </si>
-  <si>
     <t>1819</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>1958</t>
+  </si>
+  <si>
+    <t>subhed</t>
   </si>
   <si>
     <t>Arizona</t>
@@ -162,49 +162,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -296,7 +291,7 @@
     </row>
     <row r="3" ht="33.0" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="8"/>
@@ -877,18 +872,18 @@
         <v>7</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4">

</xml_diff>